<commit_message>
Adding sqlite container for specifications
warning: breaks stats
features are fine
</commit_message>
<xml_diff>
--- a/movement_validation/statistics/feature_metadata/features specifications.xlsx
+++ b/movement_validation/statistics/feature_metadata/features specifications.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FeatureSpecifications" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="307">
   <si>
     <t>feature_field</t>
   </si>
@@ -898,6 +898,45 @@
   </si>
   <si>
     <t>no units</t>
+  </si>
+  <si>
+    <t>The category: Morphology, Posture, Locomotion, or Path.</t>
+  </si>
+  <si>
+    <t>The full heirarchical path, delimited by periods (.)</t>
+  </si>
+  <si>
+    <t>The old sub_field in the original Schafer Lab code.</t>
+  </si>
+  <si>
+    <t>The old feature_field name in the original Schafer Lab code.</t>
+  </si>
+  <si>
+    <t>A shorter description of the feature</t>
+  </si>
+  <si>
+    <t>A longer description of the feature</t>
+  </si>
+  <si>
+    <t>AKA "resolution".  The width of the bins for the histogram.</t>
+  </si>
+  <si>
+    <t>Are negative values allowed?</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>What units the quantity is expressed in</t>
+  </si>
+  <si>
+    <t>The name of the field containing the signed data</t>
+  </si>
+  <si>
+    <t>Used only for eigen_projections: the index of the eigen_projection</t>
+  </si>
+  <si>
+    <t>Is the data a time series? (?)</t>
   </si>
 </sst>
 </file>
@@ -968,6 +1007,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1015,7 +1057,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1050,7 +1092,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1261,9 +1303,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4790,9 +4832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4829,6 +4869,9 @@
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="C3" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -4836,6 +4879,9 @@
       </c>
       <c r="B4">
         <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -4845,6 +4891,9 @@
       <c r="B5">
         <v>1</v>
       </c>
+      <c r="C5" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -4853,6 +4902,9 @@
       <c r="B6">
         <v>1</v>
       </c>
+      <c r="C6" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -4861,6 +4913,9 @@
       <c r="B7">
         <v>1</v>
       </c>
+      <c r="C7" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -4869,6 +4924,9 @@
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -4876,6 +4934,9 @@
       </c>
       <c r="B9">
         <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -4885,6 +4946,9 @@
       <c r="B10">
         <v>4</v>
       </c>
+      <c r="C10" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -4893,6 +4957,9 @@
       <c r="B11">
         <v>4</v>
       </c>
+      <c r="C11" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -4901,21 +4968,42 @@
       <c r="B12">
         <v>1</v>
       </c>
+      <c r="C12" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -4924,16 +5012,22 @@
       <c r="B16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -4941,7 +5035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -4949,7 +5043,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -4957,7 +5051,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3</v>
       </c>
@@ -4965,7 +5059,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>

</xml_diff>